<commit_message>
Selenium and TestNG baseTest class
</commit_message>
<xml_diff>
--- a/bin/data.xlsx
+++ b/bin/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codebase\UISpiceJet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0020381-9D80-49F2-9F1D-09F314A040AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F001587-BE72-4193-9C7E-F408991A125B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AE0F00E8-335A-451B-BA26-FE26354170E2}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>